<commit_message>
reran import_orgs to ensure the aparna tag is within tags
</commit_message>
<xml_diff>
--- a/scripts/users_list.xlsx
+++ b/scripts/users_list.xlsx
@@ -403,1027 +403,1027 @@
     <t>3Cinteractive</t>
   </si>
   <si>
-    <t>Jennifer Hansen - CE - aparna</t>
-  </si>
-  <si>
-    <t>Kate Hoffman - CE - aparna</t>
-  </si>
-  <si>
-    <t>Anna Dalby - CE - aparna</t>
-  </si>
-  <si>
-    <t>Aubrey Kaine - CE - aparna</t>
-  </si>
-  <si>
-    <t>Francis Kind - CE - aparna</t>
-  </si>
-  <si>
-    <t>Bunk Moreland - CE - aparna</t>
-  </si>
-  <si>
-    <t>Lester Freamon - CE - aparna</t>
-  </si>
-  <si>
-    <t>Marlo Stanfield - CE - aparna</t>
-  </si>
-  <si>
-    <t>Emma Lee - CE - aparna</t>
-  </si>
-  <si>
-    <t>Shirin Poeplinghaus - CE - aparna</t>
-  </si>
-  <si>
-    <t>Jimmy McNulty - CE - aparna</t>
-  </si>
-  <si>
-    <t>Lisa Roth - CE - aparna</t>
-  </si>
-  <si>
-    <t>Sample customer - aparna</t>
-  </si>
-  <si>
-    <t>Em Cino - CE - aparna</t>
-  </si>
-  <si>
-    <t>Samira Miller - CE - aparna</t>
-  </si>
-  <si>
-    <t>Karen Biscopink - CE - aparna</t>
-  </si>
-  <si>
-    <t>Robert - aparna</t>
-  </si>
-  <si>
-    <t>Jen Doe - CE - aparna</t>
-  </si>
-  <si>
-    <t>Charles Nadeau - CE - aparna</t>
-  </si>
-  <si>
-    <t>Laduma Nguyuza - aparna</t>
-  </si>
-  <si>
-    <t>Fred Flora - CE - aparna</t>
-  </si>
-  <si>
-    <t>Jackson Davis - CE - aparna</t>
-  </si>
-  <si>
-    <t>Megan Browning - CE - aparna</t>
-  </si>
-  <si>
-    <t>Mark Banuelos - CE - aparna</t>
-  </si>
-  <si>
-    <t>Clark Green - CE - aparna</t>
-  </si>
-  <si>
-    <t>Nick Lopez - aparna</t>
-  </si>
-  <si>
-    <t>Alexander Migale - CE - aparna</t>
-  </si>
-  <si>
-    <t>Beatrix Abbott - CE - aparna</t>
-  </si>
-  <si>
-    <t>Cruz Smith - CE - aparna</t>
-  </si>
-  <si>
-    <t>Courtney Benjamin-CE - aparna</t>
-  </si>
-  <si>
-    <t>Austin Haukinz - CE - aparna</t>
-  </si>
-  <si>
-    <t>Aza Coward - CE - aparna</t>
-  </si>
-  <si>
-    <t>Eat Well Support - aparna</t>
-  </si>
-  <si>
-    <t>Malcom - aparna</t>
-  </si>
-  <si>
-    <t>Chris Meyers - aparna</t>
-  </si>
-  <si>
-    <t>John Smith - aparna</t>
-  </si>
-  <si>
-    <t>george - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 23590364 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 96375178 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 7277679 - aparna</t>
-  </si>
-  <si>
-    <t>Test - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 88770589 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 56361663 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 44363997 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 79609699 - aparna</t>
-  </si>
-  <si>
-    <t>George - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 86361647 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 9069214 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 33491187 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 42889124 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 85664065 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 11995833 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 17497796 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 26613524 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 56042054 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 14343384 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 13789444 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 87985401 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 14272733 - aparna</t>
-  </si>
-  <si>
-    <t>Efren - aparna</t>
-  </si>
-  <si>
-    <t>Sera Tajima - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 41764726 - aparna</t>
-  </si>
-  <si>
-    <t>Shirin - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 64655414 - aparna</t>
-  </si>
-  <si>
-    <t>Caller Unknown - aparna</t>
-  </si>
-  <si>
-    <t>Amanda Gamblin - CE - aparna</t>
-  </si>
-  <si>
-    <t>Agamblintest - aparna</t>
-  </si>
-  <si>
-    <t>Laurence Hardie - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 85725979 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 64846162 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 72934791 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 80224582 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 17565537 - aparna</t>
-  </si>
-  <si>
-    <t>Sam Smitty - aparna</t>
-  </si>
-  <si>
-    <t>65092144444_flagged_for_inspection - aparna</t>
-  </si>
-  <si>
-    <t>Benoit Duval - aparna</t>
-  </si>
-  <si>
-    <t>Jane Smith - aparna</t>
-  </si>
-  <si>
-    <t>Leister - aparna</t>
-  </si>
-  <si>
-    <t>1 707 553-3856 - aparna</t>
-  </si>
-  <si>
-    <t>Liz Roth - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 608 628-4363 - aparna</t>
-  </si>
-  <si>
-    <t>Qwerty - aparna</t>
-  </si>
-  <si>
-    <t>Cookie Monster - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 17886942 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 81100780 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 86431441 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 9729838 - aparna</t>
-  </si>
-  <si>
-    <t>Tom Cruise - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 310 897-9537 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 353 87 352 5778 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 92968055 - aparna</t>
-  </si>
-  <si>
-    <t>Text user: 61429565663 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 56053843 - aparna</t>
-  </si>
-  <si>
-    <t>Customer Name - aparna</t>
-  </si>
-  <si>
-    <t>Henry Block - aparna</t>
-  </si>
-  <si>
-    <t>Tom Smith - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 51823672 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 80254017 - aparna</t>
-  </si>
-  <si>
-    <t>Bob Smith - aparna</t>
-  </si>
-  <si>
-    <t>Silvia Mueller - aparna</t>
-  </si>
-  <si>
-    <t>Leo Steim - aparna</t>
-  </si>
-  <si>
-    <t>Fabian Flor - aparna</t>
-  </si>
-  <si>
-    <t>Mark Smith - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 11789822 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 89800926 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 85313381 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 55191318 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 52158329 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 415 653-0291 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 415 449-7593 - aparna</t>
-  </si>
-  <si>
-    <t>René F. Lisi - aparna</t>
-  </si>
-  <si>
-    <t>Sara Gholampour - CE - aparna</t>
-  </si>
-  <si>
-    <t>Andy J - aparna</t>
-  </si>
-  <si>
-    <t>Mary Poeplinghaus - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 71862868 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 74360839 - aparna</t>
-  </si>
-  <si>
-    <t>Stephanie Pellegrino - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 90093682 - aparna</t>
-  </si>
-  <si>
-    <t>Robert Smith - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 96208453 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 66678920 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 33560748 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 51955624 - aparna</t>
-  </si>
-  <si>
-    <t>Austin Example - aparna</t>
-  </si>
-  <si>
-    <t>Jim Carrey - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 45740320 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 68618381 - aparna</t>
-  </si>
-  <si>
-    <t>James Smith - aparna</t>
-  </si>
-  <si>
-    <t>Clark Kent - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 23124403 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 2178359 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 20722305 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 59350619 - aparna</t>
-  </si>
-  <si>
-    <t>Laurence Hardie - aparna</t>
-  </si>
-  <si>
-    <t>INTERNAL Aza - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 37642204 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 54490895 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 80562267 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 70192527 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 29751713 - aparna</t>
-  </si>
-  <si>
-    <t>John Cruz - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 90758725 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 28141507 - aparna</t>
-  </si>
-  <si>
-    <t>Amanda Parker - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 1524816810 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 3070227 - aparna</t>
-  </si>
-  <si>
-    <t>Della Kartessan - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 75987045 - aparna</t>
-  </si>
-  <si>
-    <t>Thomas Paul - aparna</t>
-  </si>
-  <si>
-    <t>Megan - aparna</t>
-  </si>
-  <si>
-    <t>Text user: 61419351670 - aparna</t>
-  </si>
-  <si>
-    <t>Text user: 61432370089 - aparna</t>
-  </si>
-  <si>
-    <t>Trash End USer - aparna</t>
-  </si>
-  <si>
-    <t>Anyemailhere - aparna</t>
-  </si>
-  <si>
-    <t>Nicole Foxworth - aparna</t>
-  </si>
-  <si>
-    <t>Caller 44 20 8068 5829 - aparna</t>
-  </si>
-  <si>
-    <t>Maggie McGinnis - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 65932330 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 81779164 - aparna</t>
-  </si>
-  <si>
-    <t>Danica Beaniza - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 77710488 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 30098570 - aparna</t>
-  </si>
-  <si>
-    <t>Fashion Fan - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 60587126 - aparna</t>
-  </si>
-  <si>
-    <t>Mark Banuelos - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 38482122 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 8901240 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 19811473 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 62704675 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 64817955 - aparna</t>
-  </si>
-  <si>
-    <t>Tim - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 16879696 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 50013801 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 9425483 - aparna</t>
-  </si>
-  <si>
-    <t>Jackie - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 33536861 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 11296330 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 36380365 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 65067750 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 66768566 - aparna</t>
-  </si>
-  <si>
-    <t>Evan Felker - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 94290488 - aparna</t>
-  </si>
-  <si>
-    <t>Ivan - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 30092060 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 353 83 163 4311 - aparna</t>
-  </si>
-  <si>
-    <t>Noreply - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 13225194 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 36464076 - aparna</t>
-  </si>
-  <si>
-    <t>Coupons.com - aparna</t>
-  </si>
-  <si>
-    <t>Kelly Star - aparna</t>
-  </si>
-  <si>
-    <t>Caller 353 1 691 7262 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 72297896 - aparna</t>
-  </si>
-  <si>
-    <t>Peetnik Rewards - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 46442722 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 23887137 - aparna</t>
-  </si>
-  <si>
-    <t>Juan Cruz - aparna</t>
-  </si>
-  <si>
-    <t>Roberto Aiello - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 1534128820 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 15475841 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 61 478 367 754 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 1534133467 - aparna</t>
-  </si>
-  <si>
-    <t>Text user: 6598372254 - aparna</t>
-  </si>
-  <si>
-    <t>Jane - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 93151541 - aparna</t>
-  </si>
-  <si>
-    <t>Hubert Miller - aparna</t>
-  </si>
-  <si>
-    <t>Bonnie Leib - aparna</t>
-  </si>
-  <si>
-    <t>Mary - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 80348219 - aparna</t>
-  </si>
-  <si>
-    <t>megan - aparna</t>
-  </si>
-  <si>
-    <t>Testing User - aparna</t>
-  </si>
-  <si>
-    <t>Hubert Müller - aparna</t>
-  </si>
-  <si>
-    <t>Jane Dough - CE - aparna</t>
-  </si>
-  <si>
-    <t>Ken Copeland - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 34397965 - aparna</t>
-  </si>
-  <si>
-    <t>Maury Povach - aparna</t>
-  </si>
-  <si>
-    <t>Kale Chip - CE - aparna</t>
-  </si>
-  <si>
-    <t>Joana Ferreira - CE - aparna</t>
-  </si>
-  <si>
-    <t>Sally - aparna</t>
-  </si>
-  <si>
-    <t>Alice - aparna</t>
-  </si>
-  <si>
-    <t>George Miller - aparna</t>
-  </si>
-  <si>
-    <t>John Smythe - aparna</t>
-  </si>
-  <si>
-    <t>Laurence - aparna</t>
-  </si>
-  <si>
-    <t>John Example - aparna</t>
-  </si>
-  <si>
-    <t>Sara Gholampour - aparna</t>
-  </si>
-  <si>
-    <t>Cait Glass - aparna</t>
-  </si>
-  <si>
-    <t>Insoo Young - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 49508977 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 37980980 - aparna</t>
-  </si>
-  <si>
-    <t>Mary Miller - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 47731621 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 45821848 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 67246172 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 656 817-5970 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 80479029 - aparna</t>
-  </si>
-  <si>
-    <t>Juan Smith - aparna</t>
-  </si>
-  <si>
-    <t>Susie Williams - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 51608988 - aparna</t>
-  </si>
-  <si>
-    <t>aza says... - aparna</t>
-  </si>
-  <si>
-    <t>Ruth Cockshott - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 91877377 - aparna</t>
-  </si>
-  <si>
-    <t>Fake Customer - aparna</t>
-  </si>
-  <si>
-    <t>Wallace Example - aparna</t>
-  </si>
-  <si>
-    <t>Wallace Wears - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 47300528 - aparna</t>
-  </si>
-  <si>
-    <t>Laura Adams - CE - aparna</t>
-  </si>
-  <si>
-    <t>Ferdi Joannis - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 62157506 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 23270136 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 97813388 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 46214649 - aparna</t>
-  </si>
-  <si>
-    <t>Jeshadp - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 41363249 - aparna</t>
-  </si>
-  <si>
-    <t>Chloe Customer - Laura CE - aparna</t>
-  </si>
-  <si>
-    <t>Paul Geraghty - CE - aparna</t>
-  </si>
-  <si>
-    <t>Luke Hadley92 - aparna</t>
-  </si>
-  <si>
-    <t>Jpalkhiwalla - aparna</t>
-  </si>
-  <si>
-    <t>Matteoberin - aparna</t>
-  </si>
-  <si>
-    <t>Frank Murray - aparna</t>
-  </si>
-  <si>
-    <t>Malachi Briggs - aparna</t>
-  </si>
-  <si>
-    <t>Sara Libra - aparna</t>
-  </si>
-  <si>
-    <t>Sow Tang - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 22509194 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 62184340 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 45596237 - aparna</t>
-  </si>
-  <si>
-    <t>Dbee - aparna</t>
-  </si>
-  <si>
-    <t>1 970 819-5246 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 64987340 - aparna</t>
-  </si>
-  <si>
-    <t>Hello - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 78113833 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 71345929 - aparna</t>
-  </si>
-  <si>
-    <t>Amanda Editor - aparna</t>
-  </si>
-  <si>
-    <t>Diana - aparna</t>
-  </si>
-  <si>
-    <t>Smove Customer - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 16019904 - aparna</t>
-  </si>
-  <si>
-    <t>Fabio Guarrasi - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 6752713 - aparna</t>
-  </si>
-  <si>
-    <t>Ford Dealership L.A. - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 89762738 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 53772329 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 29123615 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 33745935 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 86104276 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 86143413 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 36763002 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 16157568 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 353 85 821 9003 - aparna</t>
-  </si>
-  <si>
-    <t>Kaitlyn Skalet - aparna</t>
-  </si>
-  <si>
-    <t>Amanda Jones - aparna</t>
-  </si>
-  <si>
-    <t>Peter Agent - aparna</t>
-  </si>
-  <si>
-    <t>Amanda Yu - CE - aparna</t>
-  </si>
-  <si>
-    <t>Dinky Skalet - CE - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 90064273 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 6435951 - aparna</t>
-  </si>
-  <si>
-    <t>Dwight Schrute - CE - aparna</t>
-  </si>
-  <si>
-    <t>Tommy Bahama - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 707 701-3321 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 35998615 - aparna</t>
-  </si>
-  <si>
-    <t>RT - aparna</t>
-  </si>
-  <si>
-    <t>Mdbeaniza - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 801 268-0727 - aparna</t>
-  </si>
-  <si>
-    <t>Btillon246 - aparna</t>
-  </si>
-  <si>
-    <t>No Email - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 24342869 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 33 6 99 63 65 78 - aparna</t>
-  </si>
-  <si>
-    <t>44 7833 591325 - aparna</t>
-  </si>
-  <si>
-    <t>Dotty Dumpling - CE - aparna</t>
-  </si>
-  <si>
-    <t>raiello@zendesk.com - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 96067358 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 42468770 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 69552426 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 68332357 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 61583225 - aparna</t>
-  </si>
-  <si>
-    <t>Laura Scrimshaw - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 75877319 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 353 87 954 1162 - aparna</t>
-  </si>
-  <si>
-    <t>Anyemailaddress - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 39653357 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 95601420 - aparna</t>
-  </si>
-  <si>
-    <t>Adam Meehan - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 2878374 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 90901574 - aparna</t>
-  </si>
-  <si>
-    <t>Jesse - aparna</t>
-  </si>
-  <si>
-    <t>Paul Geraghty - aparna</t>
-  </si>
-  <si>
-    <t>Ken Copeland - aparna</t>
-  </si>
-  <si>
-    <t>Chloe Customer - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 14363488 - aparna</t>
-  </si>
-  <si>
-    <t>Fred Flintstone - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 62892710 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 31298744 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 32146013 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 3510063 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 920 427-2381 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 56987079 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 30028211 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 47060547 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 93468409 - aparna</t>
-  </si>
-  <si>
-    <t>Caller 1 914 522-3028 - aparna</t>
-  </si>
-  <si>
-    <t>Hi - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 57164535 - aparna</t>
-  </si>
-  <si>
-    <t>Visitor 36815357 - aparna</t>
-  </si>
-  <si>
-    <t>james - aparna</t>
+    <t>Jennifer Hansen - CE</t>
+  </si>
+  <si>
+    <t>Kate Hoffman - CE</t>
+  </si>
+  <si>
+    <t>Anna Dalby - CE</t>
+  </si>
+  <si>
+    <t>Aubrey Kaine - CE</t>
+  </si>
+  <si>
+    <t>Francis Kind - CE</t>
+  </si>
+  <si>
+    <t>Bunk Moreland - CE</t>
+  </si>
+  <si>
+    <t>Lester Freamon - CE</t>
+  </si>
+  <si>
+    <t>Marlo Stanfield - CE</t>
+  </si>
+  <si>
+    <t>Emma Lee - CE</t>
+  </si>
+  <si>
+    <t>Shirin Poeplinghaus - CE</t>
+  </si>
+  <si>
+    <t>Jimmy McNulty - CE</t>
+  </si>
+  <si>
+    <t>Lisa Roth - CE</t>
+  </si>
+  <si>
+    <t>Sample customer</t>
+  </si>
+  <si>
+    <t>Em Cino - CE</t>
+  </si>
+  <si>
+    <t>Samira Miller - CE</t>
+  </si>
+  <si>
+    <t>Karen Biscopink - CE</t>
+  </si>
+  <si>
+    <t>Robert</t>
+  </si>
+  <si>
+    <t>Jen Doe - CE</t>
+  </si>
+  <si>
+    <t>Charles Nadeau - CE</t>
+  </si>
+  <si>
+    <t>Laduma Nguyuza</t>
+  </si>
+  <si>
+    <t>Fred Flora - CE</t>
+  </si>
+  <si>
+    <t>Jackson Davis - CE</t>
+  </si>
+  <si>
+    <t>Megan Browning - CE</t>
+  </si>
+  <si>
+    <t>Mark Banuelos - CE</t>
+  </si>
+  <si>
+    <t>Clark Green - CE</t>
+  </si>
+  <si>
+    <t>Nick Lopez</t>
+  </si>
+  <si>
+    <t>Alexander Migale - CE</t>
+  </si>
+  <si>
+    <t>Beatrix Abbott - CE</t>
+  </si>
+  <si>
+    <t>Cruz Smith - CE</t>
+  </si>
+  <si>
+    <t>Courtney Benjamin-CE</t>
+  </si>
+  <si>
+    <t>Austin Haukinz - CE</t>
+  </si>
+  <si>
+    <t>Aza Coward - CE</t>
+  </si>
+  <si>
+    <t>Eat Well Support</t>
+  </si>
+  <si>
+    <t>Malcom</t>
+  </si>
+  <si>
+    <t>Chris Meyers</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>george</t>
+  </si>
+  <si>
+    <t>Visitor 23590364</t>
+  </si>
+  <si>
+    <t>Visitor 96375178</t>
+  </si>
+  <si>
+    <t>Visitor 7277679</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>Visitor 88770589</t>
+  </si>
+  <si>
+    <t>Visitor 56361663</t>
+  </si>
+  <si>
+    <t>Visitor 44363997</t>
+  </si>
+  <si>
+    <t>Visitor 79609699</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>Visitor 86361647</t>
+  </si>
+  <si>
+    <t>Visitor 9069214</t>
+  </si>
+  <si>
+    <t>Visitor 33491187</t>
+  </si>
+  <si>
+    <t>Visitor 42889124</t>
+  </si>
+  <si>
+    <t>Visitor 85664065</t>
+  </si>
+  <si>
+    <t>Visitor 11995833</t>
+  </si>
+  <si>
+    <t>Visitor 17497796</t>
+  </si>
+  <si>
+    <t>Visitor 26613524</t>
+  </si>
+  <si>
+    <t>Visitor 56042054</t>
+  </si>
+  <si>
+    <t>Visitor 14343384</t>
+  </si>
+  <si>
+    <t>Visitor 13789444</t>
+  </si>
+  <si>
+    <t>Visitor 87985401</t>
+  </si>
+  <si>
+    <t>Visitor 14272733</t>
+  </si>
+  <si>
+    <t>Efren</t>
+  </si>
+  <si>
+    <t>Sera Tajima - CE</t>
+  </si>
+  <si>
+    <t>Visitor 41764726</t>
+  </si>
+  <si>
+    <t>Shirin</t>
+  </si>
+  <si>
+    <t>Visitor 64655414</t>
+  </si>
+  <si>
+    <t>Caller Unknown</t>
+  </si>
+  <si>
+    <t>Amanda Gamblin - CE</t>
+  </si>
+  <si>
+    <t>Agamblintest</t>
+  </si>
+  <si>
+    <t>Laurence Hardie - CE</t>
+  </si>
+  <si>
+    <t>Visitor 85725979</t>
+  </si>
+  <si>
+    <t>Visitor 64846162</t>
+  </si>
+  <si>
+    <t>Visitor 72934791</t>
+  </si>
+  <si>
+    <t>Visitor 80224582</t>
+  </si>
+  <si>
+    <t>Visitor 17565537</t>
+  </si>
+  <si>
+    <t>Sam Smitty</t>
+  </si>
+  <si>
+    <t>65092144444_flagged_for_inspection</t>
+  </si>
+  <si>
+    <t>Benoit Duval</t>
+  </si>
+  <si>
+    <t>Jane Smith</t>
+  </si>
+  <si>
+    <t>Leister</t>
+  </si>
+  <si>
+    <t>1 707 553-3856</t>
+  </si>
+  <si>
+    <t>Liz Roth</t>
+  </si>
+  <si>
+    <t>Caller 1 608 628-4363</t>
+  </si>
+  <si>
+    <t>Qwerty</t>
+  </si>
+  <si>
+    <t>Cookie Monster</t>
+  </si>
+  <si>
+    <t>Visitor 17886942</t>
+  </si>
+  <si>
+    <t>Visitor 81100780</t>
+  </si>
+  <si>
+    <t>Visitor 86431441</t>
+  </si>
+  <si>
+    <t>Visitor 9729838</t>
+  </si>
+  <si>
+    <t>Tom Cruise</t>
+  </si>
+  <si>
+    <t>Caller 1 310 897-9537</t>
+  </si>
+  <si>
+    <t>Caller 353 87 352 5778</t>
+  </si>
+  <si>
+    <t>Visitor 92968055</t>
+  </si>
+  <si>
+    <t>Text user: 61429565663</t>
+  </si>
+  <si>
+    <t>Visitor 56053843</t>
+  </si>
+  <si>
+    <t>Customer Name</t>
+  </si>
+  <si>
+    <t>Henry Block</t>
+  </si>
+  <si>
+    <t>Tom Smith</t>
+  </si>
+  <si>
+    <t>Visitor 51823672</t>
+  </si>
+  <si>
+    <t>Visitor 80254017</t>
+  </si>
+  <si>
+    <t>Bob Smith</t>
+  </si>
+  <si>
+    <t>Silvia Mueller</t>
+  </si>
+  <si>
+    <t>Leo Steim</t>
+  </si>
+  <si>
+    <t>Fabian Flor</t>
+  </si>
+  <si>
+    <t>Mark Smith</t>
+  </si>
+  <si>
+    <t>Visitor 11789822</t>
+  </si>
+  <si>
+    <t>Visitor 89800926</t>
+  </si>
+  <si>
+    <t>Visitor 85313381</t>
+  </si>
+  <si>
+    <t>Visitor 55191318</t>
+  </si>
+  <si>
+    <t>Visitor 52158329</t>
+  </si>
+  <si>
+    <t>Caller 1 415 653-0291</t>
+  </si>
+  <si>
+    <t>Caller 1 415 449-7593</t>
+  </si>
+  <si>
+    <t>René F. Lisi</t>
+  </si>
+  <si>
+    <t>Sara Gholampour - CE</t>
+  </si>
+  <si>
+    <t>Andy J</t>
+  </si>
+  <si>
+    <t>Mary Poeplinghaus</t>
+  </si>
+  <si>
+    <t>Visitor 71862868</t>
+  </si>
+  <si>
+    <t>Visitor 74360839</t>
+  </si>
+  <si>
+    <t>Stephanie Pellegrino - CE</t>
+  </si>
+  <si>
+    <t>Visitor 90093682</t>
+  </si>
+  <si>
+    <t>Robert Smith</t>
+  </si>
+  <si>
+    <t>Visitor 96208453</t>
+  </si>
+  <si>
+    <t>Visitor 66678920</t>
+  </si>
+  <si>
+    <t>Visitor 33560748</t>
+  </si>
+  <si>
+    <t>Visitor 51955624</t>
+  </si>
+  <si>
+    <t>Austin Example</t>
+  </si>
+  <si>
+    <t>Jim Carrey</t>
+  </si>
+  <si>
+    <t>Visitor 45740320</t>
+  </si>
+  <si>
+    <t>Visitor 68618381</t>
+  </si>
+  <si>
+    <t>James Smith</t>
+  </si>
+  <si>
+    <t>Clark Kent</t>
+  </si>
+  <si>
+    <t>Visitor 23124403</t>
+  </si>
+  <si>
+    <t>Visitor 2178359</t>
+  </si>
+  <si>
+    <t>Visitor 20722305</t>
+  </si>
+  <si>
+    <t>Visitor 59350619</t>
+  </si>
+  <si>
+    <t>Laurence Hardie</t>
+  </si>
+  <si>
+    <t>INTERNAL Aza</t>
+  </si>
+  <si>
+    <t>Visitor 37642204</t>
+  </si>
+  <si>
+    <t>Visitor 54490895</t>
+  </si>
+  <si>
+    <t>Visitor 80562267</t>
+  </si>
+  <si>
+    <t>Visitor 70192527</t>
+  </si>
+  <si>
+    <t>Visitor 29751713</t>
+  </si>
+  <si>
+    <t>John Cruz</t>
+  </si>
+  <si>
+    <t>Visitor 90758725</t>
+  </si>
+  <si>
+    <t>Visitor 28141507</t>
+  </si>
+  <si>
+    <t>Amanda Parker</t>
+  </si>
+  <si>
+    <t>Visitor 1524816810</t>
+  </si>
+  <si>
+    <t>Visitor 3070227</t>
+  </si>
+  <si>
+    <t>Della Kartessan - CE</t>
+  </si>
+  <si>
+    <t>Visitor 75987045</t>
+  </si>
+  <si>
+    <t>Thomas Paul</t>
+  </si>
+  <si>
+    <t>Megan</t>
+  </si>
+  <si>
+    <t>Text user: 61419351670</t>
+  </si>
+  <si>
+    <t>Text user: 61432370089</t>
+  </si>
+  <si>
+    <t>Trash End USer</t>
+  </si>
+  <si>
+    <t>Anyemailhere</t>
+  </si>
+  <si>
+    <t>Nicole Foxworth</t>
+  </si>
+  <si>
+    <t>Caller 44 20 8068 5829</t>
+  </si>
+  <si>
+    <t>Maggie McGinnis</t>
+  </si>
+  <si>
+    <t>Visitor 65932330</t>
+  </si>
+  <si>
+    <t>Visitor 81779164</t>
+  </si>
+  <si>
+    <t>Danica Beaniza - CE</t>
+  </si>
+  <si>
+    <t>Visitor 77710488</t>
+  </si>
+  <si>
+    <t>Visitor 30098570</t>
+  </si>
+  <si>
+    <t>Fashion Fan</t>
+  </si>
+  <si>
+    <t>Visitor 60587126</t>
+  </si>
+  <si>
+    <t>Mark Banuelos</t>
+  </si>
+  <si>
+    <t>Visitor 38482122</t>
+  </si>
+  <si>
+    <t>Visitor 8901240</t>
+  </si>
+  <si>
+    <t>Visitor 19811473</t>
+  </si>
+  <si>
+    <t>Visitor 62704675</t>
+  </si>
+  <si>
+    <t>Visitor 64817955</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Visitor 16879696</t>
+  </si>
+  <si>
+    <t>Visitor 50013801</t>
+  </si>
+  <si>
+    <t>Visitor 9425483</t>
+  </si>
+  <si>
+    <t>Jackie</t>
+  </si>
+  <si>
+    <t>Visitor 33536861</t>
+  </si>
+  <si>
+    <t>Visitor 11296330</t>
+  </si>
+  <si>
+    <t>Visitor 36380365</t>
+  </si>
+  <si>
+    <t>Visitor 65067750</t>
+  </si>
+  <si>
+    <t>Visitor 66768566</t>
+  </si>
+  <si>
+    <t>Evan Felker</t>
+  </si>
+  <si>
+    <t>Visitor 94290488</t>
+  </si>
+  <si>
+    <t>Ivan</t>
+  </si>
+  <si>
+    <t>Visitor 30092060</t>
+  </si>
+  <si>
+    <t>Caller 353 83 163 4311</t>
+  </si>
+  <si>
+    <t>Noreply</t>
+  </si>
+  <si>
+    <t>Visitor 13225194</t>
+  </si>
+  <si>
+    <t>Visitor 36464076</t>
+  </si>
+  <si>
+    <t>Coupons.com</t>
+  </si>
+  <si>
+    <t>Kelly Star</t>
+  </si>
+  <si>
+    <t>Caller 353 1 691 7262</t>
+  </si>
+  <si>
+    <t>Visitor 72297896</t>
+  </si>
+  <si>
+    <t>Peetnik Rewards</t>
+  </si>
+  <si>
+    <t>Visitor 46442722</t>
+  </si>
+  <si>
+    <t>Visitor 23887137</t>
+  </si>
+  <si>
+    <t>Juan Cruz</t>
+  </si>
+  <si>
+    <t>Roberto Aiello</t>
+  </si>
+  <si>
+    <t>Visitor 1534128820</t>
+  </si>
+  <si>
+    <t>Visitor 15475841</t>
+  </si>
+  <si>
+    <t>Caller 61 478 367 754</t>
+  </si>
+  <si>
+    <t>Visitor 1534133467</t>
+  </si>
+  <si>
+    <t>Text user: 6598372254</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Visitor 93151541</t>
+  </si>
+  <si>
+    <t>Hubert Miller</t>
+  </si>
+  <si>
+    <t>Bonnie Leib</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Visitor 80348219</t>
+  </si>
+  <si>
+    <t>megan</t>
+  </si>
+  <si>
+    <t>Testing User</t>
+  </si>
+  <si>
+    <t>Hubert Müller</t>
+  </si>
+  <si>
+    <t>Jane Dough - CE</t>
+  </si>
+  <si>
+    <t>Ken Copeland - CE</t>
+  </si>
+  <si>
+    <t>Visitor 34397965</t>
+  </si>
+  <si>
+    <t>Maury Povach</t>
+  </si>
+  <si>
+    <t>Kale Chip - CE</t>
+  </si>
+  <si>
+    <t>Joana Ferreira - CE</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>George Miller</t>
+  </si>
+  <si>
+    <t>John Smythe</t>
+  </si>
+  <si>
+    <t>Laurence</t>
+  </si>
+  <si>
+    <t>John Example</t>
+  </si>
+  <si>
+    <t>Sara Gholampour</t>
+  </si>
+  <si>
+    <t>Cait Glass</t>
+  </si>
+  <si>
+    <t>Insoo Young</t>
+  </si>
+  <si>
+    <t>Visitor 49508977</t>
+  </si>
+  <si>
+    <t>Visitor 37980980</t>
+  </si>
+  <si>
+    <t>Mary Miller</t>
+  </si>
+  <si>
+    <t>Visitor 47731621</t>
+  </si>
+  <si>
+    <t>Visitor 45821848</t>
+  </si>
+  <si>
+    <t>Visitor 67246172</t>
+  </si>
+  <si>
+    <t>Caller 1 656 817-5970</t>
+  </si>
+  <si>
+    <t>Visitor 80479029</t>
+  </si>
+  <si>
+    <t>Juan Smith</t>
+  </si>
+  <si>
+    <t>Susie Williams</t>
+  </si>
+  <si>
+    <t>Visitor 51608988</t>
+  </si>
+  <si>
+    <t>aza says...</t>
+  </si>
+  <si>
+    <t>Ruth Cockshott</t>
+  </si>
+  <si>
+    <t>Visitor 91877377</t>
+  </si>
+  <si>
+    <t>Fake Customer</t>
+  </si>
+  <si>
+    <t>Wallace Example</t>
+  </si>
+  <si>
+    <t>Wallace Wears</t>
+  </si>
+  <si>
+    <t>Visitor 47300528</t>
+  </si>
+  <si>
+    <t>Laura Adams - CE</t>
+  </si>
+  <si>
+    <t>Ferdi Joannis</t>
+  </si>
+  <si>
+    <t>Visitor 62157506</t>
+  </si>
+  <si>
+    <t>Visitor 23270136</t>
+  </si>
+  <si>
+    <t>Visitor 97813388</t>
+  </si>
+  <si>
+    <t>Visitor 46214649</t>
+  </si>
+  <si>
+    <t>Jeshadp</t>
+  </si>
+  <si>
+    <t>Visitor 41363249</t>
+  </si>
+  <si>
+    <t>Chloe Customer - Laura CE</t>
+  </si>
+  <si>
+    <t>Paul Geraghty - CE</t>
+  </si>
+  <si>
+    <t>Luke Hadley92</t>
+  </si>
+  <si>
+    <t>Jpalkhiwalla</t>
+  </si>
+  <si>
+    <t>Matteoberin</t>
+  </si>
+  <si>
+    <t>Frank Murray</t>
+  </si>
+  <si>
+    <t>Malachi Briggs</t>
+  </si>
+  <si>
+    <t>Sara Libra</t>
+  </si>
+  <si>
+    <t>Sow Tang</t>
+  </si>
+  <si>
+    <t>Visitor 22509194</t>
+  </si>
+  <si>
+    <t>Visitor 62184340</t>
+  </si>
+  <si>
+    <t>Visitor 45596237</t>
+  </si>
+  <si>
+    <t>Dbee</t>
+  </si>
+  <si>
+    <t>1 970 819-5246</t>
+  </si>
+  <si>
+    <t>Visitor 64987340</t>
+  </si>
+  <si>
+    <t>Hello</t>
+  </si>
+  <si>
+    <t>Visitor 78113833</t>
+  </si>
+  <si>
+    <t>Visitor 71345929</t>
+  </si>
+  <si>
+    <t>Amanda Editor</t>
+  </si>
+  <si>
+    <t>Diana</t>
+  </si>
+  <si>
+    <t>Smove Customer</t>
+  </si>
+  <si>
+    <t>Visitor 16019904</t>
+  </si>
+  <si>
+    <t>Fabio Guarrasi</t>
+  </si>
+  <si>
+    <t>Visitor 6752713</t>
+  </si>
+  <si>
+    <t>Ford Dealership L.A.</t>
+  </si>
+  <si>
+    <t>Visitor 89762738</t>
+  </si>
+  <si>
+    <t>Visitor 53772329</t>
+  </si>
+  <si>
+    <t>Visitor 29123615</t>
+  </si>
+  <si>
+    <t>Visitor 33745935</t>
+  </si>
+  <si>
+    <t>Visitor 86104276</t>
+  </si>
+  <si>
+    <t>Visitor 86143413</t>
+  </si>
+  <si>
+    <t>Visitor 36763002</t>
+  </si>
+  <si>
+    <t>Visitor 16157568</t>
+  </si>
+  <si>
+    <t>Caller 353 85 821 9003</t>
+  </si>
+  <si>
+    <t>Kaitlyn Skalet</t>
+  </si>
+  <si>
+    <t>Amanda Jones</t>
+  </si>
+  <si>
+    <t>Peter Agent</t>
+  </si>
+  <si>
+    <t>Amanda Yu - CE</t>
+  </si>
+  <si>
+    <t>Dinky Skalet - CE</t>
+  </si>
+  <si>
+    <t>Visitor 90064273</t>
+  </si>
+  <si>
+    <t>Visitor 6435951</t>
+  </si>
+  <si>
+    <t>Dwight Schrute - CE</t>
+  </si>
+  <si>
+    <t>Tommy Bahama</t>
+  </si>
+  <si>
+    <t>Caller 1 707 701-3321</t>
+  </si>
+  <si>
+    <t>Visitor 35998615</t>
+  </si>
+  <si>
+    <t>RT</t>
+  </si>
+  <si>
+    <t>Mdbeaniza</t>
+  </si>
+  <si>
+    <t>Caller 1 801 268-0727</t>
+  </si>
+  <si>
+    <t>Btillon246</t>
+  </si>
+  <si>
+    <t>No Email</t>
+  </si>
+  <si>
+    <t>Visitor 24342869</t>
+  </si>
+  <si>
+    <t>Caller 33 6 99 63 65 78</t>
+  </si>
+  <si>
+    <t>44 7833 591325</t>
+  </si>
+  <si>
+    <t>Dotty Dumpling - CE</t>
+  </si>
+  <si>
+    <t>raiello@zendesk.com</t>
+  </si>
+  <si>
+    <t>Visitor 96067358</t>
+  </si>
+  <si>
+    <t>Visitor 42468770</t>
+  </si>
+  <si>
+    <t>Visitor 69552426</t>
+  </si>
+  <si>
+    <t>Visitor 68332357</t>
+  </si>
+  <si>
+    <t>Visitor 61583225</t>
+  </si>
+  <si>
+    <t>Laura Scrimshaw</t>
+  </si>
+  <si>
+    <t>Visitor 75877319</t>
+  </si>
+  <si>
+    <t>Caller 353 87 954 1162</t>
+  </si>
+  <si>
+    <t>Anyemailaddress</t>
+  </si>
+  <si>
+    <t>Visitor 39653357</t>
+  </si>
+  <si>
+    <t>Visitor 95601420</t>
+  </si>
+  <si>
+    <t>Adam Meehan</t>
+  </si>
+  <si>
+    <t>Visitor 2878374</t>
+  </si>
+  <si>
+    <t>Visitor 90901574</t>
+  </si>
+  <si>
+    <t>Jesse</t>
+  </si>
+  <si>
+    <t>Paul Geraghty</t>
+  </si>
+  <si>
+    <t>Ken Copeland</t>
+  </si>
+  <si>
+    <t>Chloe Customer</t>
+  </si>
+  <si>
+    <t>Visitor 14363488</t>
+  </si>
+  <si>
+    <t>Fred Flintstone</t>
+  </si>
+  <si>
+    <t>Visitor 62892710</t>
+  </si>
+  <si>
+    <t>Visitor 31298744</t>
+  </si>
+  <si>
+    <t>Visitor 32146013</t>
+  </si>
+  <si>
+    <t>Visitor 3510063</t>
+  </si>
+  <si>
+    <t>Caller 1 920 427-2381</t>
+  </si>
+  <si>
+    <t>Visitor 56987079</t>
+  </si>
+  <si>
+    <t>Visitor 30028211</t>
+  </si>
+  <si>
+    <t>Visitor 47060547</t>
+  </si>
+  <si>
+    <t>Visitor 93468409</t>
+  </si>
+  <si>
+    <t>Caller 1 914 522-3028</t>
+  </si>
+  <si>
+    <t>Hi</t>
+  </si>
+  <si>
+    <t>Visitor 57164535</t>
+  </si>
+  <si>
+    <t>Visitor 36815357</t>
+  </si>
+  <si>
+    <t>james</t>
   </si>
   <si>
     <t>jhansen@example.com</t>
@@ -1879,20 +1879,20 @@
     <t>agent</t>
   </si>
   <si>
-    <t xml:space="preserve">Likes emojis </t>
+    <t>Likes emojis 😊</t>
   </si>
   <si>
     <t>Here are some notes about Clark
 8/9/18 - More notes</t>
   </si>
   <si>
-    <t>Azas End User</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Big fan of honey </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mmmm donuts </t>
+    <t>Aza's 'End User'</t>
+  </si>
+  <si>
+    <t>Big fan of honey 🐝</t>
+  </si>
+  <si>
+    <t>Mmmm donuts 🍩</t>
   </si>
   <si>
     <t>Advanced Support - CE</t>
@@ -1913,16 +1913,16 @@
     <t>Promotions - CE</t>
   </si>
   <si>
-    <t>planunderscoregold</t>
-  </si>
-  <si>
-    <t>planunderscoresilver</t>
-  </si>
-  <si>
-    <t>planunderscorebronze</t>
-  </si>
-  <si>
-    <t>planunderscoreplatinum</t>
+    <t>plan_gold</t>
+  </si>
+  <si>
+    <t>plan_silver</t>
+  </si>
+  <si>
+    <t>plan_bronze</t>
+  </si>
+  <si>
+    <t>plan_platinum</t>
   </si>
   <si>
     <t>doloratdoloremque</t>
@@ -2945,67 +2945,67 @@
     <t>totamdolorsequi</t>
   </si>
   <si>
-    <t>[]</t>
-  </si>
-  <si>
-    <t>['subscriptionunderscoresilver', 'productunderscorea', 'chefunderscoredequipe', 'planunderscoregold', 'nounderscorecsat']</t>
-  </si>
-  <si>
-    <t>['gold', 'paid', 'sanunderscorefrancisco', 'co-op', 'vip']</t>
-  </si>
-  <si>
-    <t>['planunderscoregold', 'vipunderscoreuser', 'nounderscorecsat']</t>
-  </si>
-  <si>
-    <t>['tier1underscoresupport']</t>
-  </si>
-  <si>
-    <t>['vipunderscoreuser', 'emea', 'planunderscoresilver', 'resigned']</t>
-  </si>
-  <si>
-    <t>['planunderscoresilver']</t>
-  </si>
-  <si>
-    <t>['planunderscoregold', 'nounderscorecsat']</t>
-  </si>
-  <si>
-    <t>['planunderscoresilver', 'vip']</t>
-  </si>
-  <si>
-    <t>['sales', 'training']</t>
-  </si>
-  <si>
-    <t>['gold', 'emeaunderscorecustomer', 'london', 'europe']</t>
-  </si>
-  <si>
-    <t>['guideunderscoretier1underscoresection']</t>
-  </si>
-  <si>
-    <t>['planunderscoregold']</t>
-  </si>
-  <si>
-    <t>['vip']</t>
-  </si>
-  <si>
-    <t>['planunderscoregold', 'vip']</t>
-  </si>
-  <si>
-    <t>['resigned', 'planunderscoregold']</t>
-  </si>
-  <si>
-    <t>['east', 'vip']</t>
-  </si>
-  <si>
-    <t>['vipunderscoreuser', 'planunderscoregold']</t>
-  </si>
-  <si>
-    <t>['emea', 'eatwellunderscoreemployee']</t>
-  </si>
-  <si>
-    <t>['editor']</t>
-  </si>
-  <si>
-    <t>['itmanager']</t>
+    <t>aparna</t>
+  </si>
+  <si>
+    <t>subscription_silver, product_a, chef_dequipe, plan_gold, no_csat, aparna</t>
+  </si>
+  <si>
+    <t>gold, paid, san_francisco, co-op, vip, aparna</t>
+  </si>
+  <si>
+    <t>plan_gold, vip_user, no_csat, aparna</t>
+  </si>
+  <si>
+    <t>tier1_support, aparna</t>
+  </si>
+  <si>
+    <t>vip_user, emea, plan_silver, resigned, aparna</t>
+  </si>
+  <si>
+    <t>plan_silver, aparna</t>
+  </si>
+  <si>
+    <t>plan_gold, no_csat, aparna</t>
+  </si>
+  <si>
+    <t>plan_silver, vip, aparna</t>
+  </si>
+  <si>
+    <t>sales, training, aparna</t>
+  </si>
+  <si>
+    <t>gold, emea_customer, london, europe, aparna</t>
+  </si>
+  <si>
+    <t>guide_tier1_section, aparna</t>
+  </si>
+  <si>
+    <t>plan_gold, aparna</t>
+  </si>
+  <si>
+    <t>vip, aparna</t>
+  </si>
+  <si>
+    <t>plan_gold, vip, aparna</t>
+  </si>
+  <si>
+    <t>resigned, plan_gold, aparna</t>
+  </si>
+  <si>
+    <t>east, vip, aparna</t>
+  </si>
+  <si>
+    <t>vip_user, plan_gold, aparna</t>
+  </si>
+  <si>
+    <t>emea, eatwell_employee, aparna</t>
+  </si>
+  <si>
+    <t>editor, aparna</t>
+  </si>
+  <si>
+    <t>itmanager, aparna</t>
   </si>
 </sst>
 </file>

</xml_diff>